<commit_message>
Updated excel sheet and length of exercise names.
</commit_message>
<xml_diff>
--- a/app/existing_data/OPT Phase Breakdown.xlsx
+++ b/app/existing_data/OPT Phase Breakdown.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3147" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3447" uniqueCount="591">
   <si>
     <t>unit</t>
   </si>
@@ -1547,6 +1547,135 @@
   </si>
   <si>
     <t>weighted step-up to balance</t>
+  </si>
+  <si>
+    <t>dumbbell ball squat</t>
+  </si>
+  <si>
+    <t>wall</t>
+  </si>
+  <si>
+    <t>dumbbell squat</t>
+  </si>
+  <si>
+    <t>resistance-stabilization &amp; resistance-strength</t>
+  </si>
+  <si>
+    <t>leg press</t>
+  </si>
+  <si>
+    <t>bilateral</t>
+  </si>
+  <si>
+    <t>hip sled</t>
+  </si>
+  <si>
+    <t>barbell back squat</t>
+  </si>
+  <si>
+    <t>single-leg dumbbell scaption</t>
+  </si>
+  <si>
+    <t>single-leg dumbbell scaption alternating arm</t>
+  </si>
+  <si>
+    <t>single-leg dumbbell scaption single arm</t>
+  </si>
+  <si>
+    <t>dumbbell scaption</t>
+  </si>
+  <si>
+    <t>seated dumbbell scaption</t>
+  </si>
+  <si>
+    <t>bench | chair</t>
+  </si>
+  <si>
+    <t>seated stability ball dumbbell scaption</t>
+  </si>
+  <si>
+    <t>seated stability ball shoulder press</t>
+  </si>
+  <si>
+    <t>seated shoulder press</t>
+  </si>
+  <si>
+    <t>seated stability ball shoulder press alternating arm</t>
+  </si>
+  <si>
+    <t>seated stability ball shoulder press single arm</t>
+  </si>
+  <si>
+    <t>seated shoulder press machine</t>
+  </si>
+  <si>
+    <t>shoulder press machine</t>
+  </si>
+  <si>
+    <t>front medicine ball oblique throw</t>
+  </si>
+  <si>
+    <t>overhead medicine ball throw</t>
+  </si>
+  <si>
+    <t>single-leg dumbbell curl</t>
+  </si>
+  <si>
+    <t>single-leg dumbbell curl alternating arm</t>
+  </si>
+  <si>
+    <t>single-leg dumbbell curl single arm</t>
+  </si>
+  <si>
+    <t>dumbbell curl</t>
+  </si>
+  <si>
+    <t>single-leg barbell curl</t>
+  </si>
+  <si>
+    <t>barbell curl</t>
+  </si>
+  <si>
+    <t>seated dumbbell biceps curl</t>
+  </si>
+  <si>
+    <t>seated stability ball biceps curl</t>
+  </si>
+  <si>
+    <t>biceps curl machine</t>
+  </si>
+  <si>
+    <t>supine ball dumbbell triceps extension</t>
+  </si>
+  <si>
+    <t>supine bench dumbbell triceps extension</t>
+  </si>
+  <si>
+    <t>supine ball dumbbell triceps extension alternating arm</t>
+  </si>
+  <si>
+    <t>supine ball dumbbell triceps extension single arm</t>
+  </si>
+  <si>
+    <t>unilateral</t>
+  </si>
+  <si>
+    <t>prone ball dumbbell triceps extensions</t>
+  </si>
+  <si>
+    <t>triceps cable pushdown</t>
+  </si>
+  <si>
+    <t>triceps cable pushdown machine</t>
+  </si>
+  <si>
+    <t>prone ball dumbbell triceps extensions alternating arm</t>
+  </si>
+  <si>
+    <t>prone ball dumbbell triceps extensions single arm</t>
+  </si>
+  <si>
+    <t>supine bench barbell triceps extension</t>
   </si>
   <si>
     <t>Sagittal; Frontal: Transverse</t>
@@ -1781,7 +1910,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1864,6 +1993,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3520,6 +3652,7 @@
     <col customWidth="1" min="9" max="12" width="17.5"/>
     <col customWidth="1" min="13" max="13" width="19.25"/>
     <col customWidth="1" min="14" max="14" width="17.38"/>
+    <col customWidth="1" min="15" max="15" width="25.13"/>
     <col customWidth="1" min="16" max="16" width="16.5"/>
     <col customWidth="1" min="17" max="17" width="18.25"/>
     <col customWidth="1" min="18" max="18" width="20.13"/>
@@ -3613,7 +3746,7 @@
         <v>2.0</v>
       </c>
       <c r="D2" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>328</v>
@@ -3652,7 +3785,7 @@
         <v>2.0</v>
       </c>
       <c r="D3" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>328</v>
@@ -3691,7 +3824,7 @@
         <v>2.0</v>
       </c>
       <c r="D4" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>328</v>
@@ -3729,7 +3862,7 @@
         <v>2.0</v>
       </c>
       <c r="D5" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>328</v>
@@ -3767,7 +3900,7 @@
         <v>2.0</v>
       </c>
       <c r="D6" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>328</v>
@@ -3806,7 +3939,7 @@
         <v>2.0</v>
       </c>
       <c r="D7" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>328</v>
@@ -7667,7 +7800,7 @@
         <v>443</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="I106" s="27"/>
       <c r="J106" s="27"/>
@@ -7796,214 +7929,1295 @@
       <c r="P109" s="1"/>
     </row>
     <row r="110">
+      <c r="A110" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C110" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="D110" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="I110" s="30"/>
       <c r="J110" s="30"/>
       <c r="K110" s="30"/>
-      <c r="L110" s="30"/>
+      <c r="L110" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="M110" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="O110" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="Q110" s="1" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="111">
+      <c r="A111" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C111" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="D111" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="I111" s="30"/>
       <c r="J111" s="30"/>
       <c r="K111" s="30"/>
-      <c r="L111" s="30"/>
+      <c r="L111" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="M111" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="O111" s="1" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="112">
+      <c r="A112" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C112" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="D112" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="I112" s="30"/>
       <c r="J112" s="30"/>
       <c r="K112" s="30"/>
-      <c r="L112" s="30"/>
+      <c r="L112" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="M112" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="O112" s="1" t="s">
+        <v>510</v>
+      </c>
     </row>
     <row r="113">
+      <c r="A113" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C113" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="D113" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="I113" s="30"/>
       <c r="J113" s="30"/>
       <c r="K113" s="30"/>
-      <c r="L113" s="30"/>
+      <c r="L113" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="M113" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="O113" s="1" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="114">
+      <c r="A114" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C114" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="D114" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="I114" s="30"/>
       <c r="J114" s="30"/>
       <c r="K114" s="30"/>
-      <c r="L114" s="30"/>
+      <c r="L114" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="M114" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="O114" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="S114" s="1" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="115">
+      <c r="A115" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C115" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="D115" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="I115" s="30"/>
       <c r="J115" s="30"/>
       <c r="K115" s="30"/>
-      <c r="L115" s="30"/>
+      <c r="L115" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="M115" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="O115" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="S115" s="1" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="116">
+      <c r="A116" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C116" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="D116" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="I116" s="30"/>
       <c r="J116" s="30"/>
       <c r="K116" s="30"/>
-      <c r="L116" s="30"/>
+      <c r="L116" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="M116" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="O116" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="S116" s="1" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="117">
+      <c r="A117" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C117" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D117" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="I117" s="30"/>
       <c r="J117" s="30"/>
       <c r="K117" s="30"/>
-      <c r="L117" s="30"/>
+      <c r="L117" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="M117" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="O117" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="S117" s="1" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="118">
+      <c r="A118" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C118" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D118" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>335</v>
+      </c>
       <c r="I118" s="30"/>
       <c r="J118" s="30"/>
       <c r="K118" s="30"/>
-      <c r="L118" s="30"/>
+      <c r="L118" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="M118" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="O118" s="1" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="119">
+      <c r="A119" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C119" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D119" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>335</v>
+      </c>
       <c r="I119" s="30"/>
       <c r="J119" s="30"/>
       <c r="K119" s="30"/>
-      <c r="L119" s="30"/>
+      <c r="L119" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="M119" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="O119" s="1" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="120">
+      <c r="A120" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C120" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D120" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>335</v>
+      </c>
       <c r="I120" s="30"/>
       <c r="J120" s="30"/>
       <c r="K120" s="30"/>
-      <c r="L120" s="30"/>
+      <c r="L120" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="M120" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="O120" s="1" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="121">
+      <c r="A121" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C121" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D121" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>335</v>
+      </c>
       <c r="I121" s="30"/>
       <c r="J121" s="30"/>
       <c r="K121" s="30"/>
-      <c r="L121" s="30"/>
+      <c r="L121" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="M121" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="O121" s="1" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="122">
+      <c r="A122" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C122" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D122" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>335</v>
+      </c>
       <c r="I122" s="30"/>
       <c r="J122" s="30"/>
       <c r="K122" s="30"/>
-      <c r="L122" s="30"/>
+      <c r="L122" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="M122" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="O122" s="1" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="123">
+      <c r="A123" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C123" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D123" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>335</v>
+      </c>
       <c r="I123" s="30"/>
       <c r="J123" s="30"/>
       <c r="K123" s="30"/>
-      <c r="L123" s="30"/>
+      <c r="L123" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="M123" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="O123" s="1" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="124">
+      <c r="A124" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C124" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D124" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G124" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>335</v>
+      </c>
       <c r="I124" s="30"/>
       <c r="J124" s="30"/>
       <c r="K124" s="30"/>
-      <c r="L124" s="30"/>
+      <c r="L124" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="M124" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="O124" s="1" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="125">
-      <c r="I125" s="30"/>
-      <c r="J125" s="30"/>
-      <c r="K125" s="30"/>
-      <c r="L125" s="30"/>
+      <c r="A125" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C125" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="D125" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="H125" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="I125" s="27"/>
+      <c r="J125" s="27"/>
+      <c r="K125" s="27"/>
+      <c r="L125" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="M125" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="N125" s="1"/>
+      <c r="O125" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="P125" s="1"/>
+      <c r="Q125" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="R125" s="1"/>
     </row>
     <row r="126">
-      <c r="I126" s="30"/>
-      <c r="J126" s="30"/>
-      <c r="K126" s="30"/>
-      <c r="L126" s="30"/>
+      <c r="A126" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C126" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="D126" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H126" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="I126" s="27"/>
+      <c r="J126" s="27"/>
+      <c r="K126" s="27"/>
+      <c r="L126" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="M126" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="N126" s="1"/>
+      <c r="O126" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="P126" s="1"/>
+      <c r="Q126" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="R126" s="1"/>
     </row>
     <row r="127">
+      <c r="A127" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C127" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="D127" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H127" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="I127" s="30"/>
       <c r="J127" s="30"/>
       <c r="K127" s="30"/>
-      <c r="L127" s="30"/>
+      <c r="L127" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="M127" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="O127" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="S127" s="1" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="128">
+      <c r="A128" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C128" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="D128" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H128" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="I128" s="30"/>
       <c r="J128" s="30"/>
       <c r="K128" s="30"/>
-      <c r="L128" s="30"/>
+      <c r="L128" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="M128" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="O128" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="S128" s="1" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="129">
+      <c r="A129" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C129" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="D129" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H129" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="I129" s="30"/>
       <c r="J129" s="30"/>
       <c r="K129" s="30"/>
-      <c r="L129" s="30"/>
+      <c r="L129" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="M129" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="O129" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="S129" s="1" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="130">
+      <c r="A130" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C130" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D130" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H130" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="I130" s="30"/>
       <c r="J130" s="30"/>
       <c r="K130" s="30"/>
-      <c r="L130" s="30"/>
+      <c r="L130" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="M130" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="O130" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="S130" s="1" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="131">
+      <c r="A131" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C131" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="D131" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H131" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="I131" s="30"/>
       <c r="J131" s="30"/>
       <c r="K131" s="30"/>
-      <c r="L131" s="30"/>
+      <c r="L131" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="M131" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="O131" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="S131" s="1" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="132">
+      <c r="A132" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C132" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="D132" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G132" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H132" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="I132" s="30"/>
       <c r="J132" s="30"/>
       <c r="K132" s="30"/>
-      <c r="L132" s="30"/>
+      <c r="L132" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="M132" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="O132" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="S132" s="1" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="133">
+      <c r="A133" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C133" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D133" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G133" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H133" s="1" t="s">
+        <v>335</v>
+      </c>
       <c r="I133" s="30"/>
       <c r="J133" s="30"/>
       <c r="K133" s="30"/>
-      <c r="L133" s="30"/>
+      <c r="L133" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="M133" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="O133" s="1" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="134">
+      <c r="A134" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C134" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D134" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H134" s="1" t="s">
+        <v>335</v>
+      </c>
       <c r="I134" s="30"/>
       <c r="J134" s="30"/>
       <c r="K134" s="30"/>
-      <c r="L134" s="30"/>
+      <c r="L134" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="M134" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="O134" s="1" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="135">
+      <c r="A135" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C135" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D135" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H135" s="1" t="s">
+        <v>335</v>
+      </c>
       <c r="I135" s="30"/>
       <c r="J135" s="30"/>
       <c r="K135" s="30"/>
-      <c r="L135" s="30"/>
+      <c r="L135" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="M135" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="O135" s="1" t="s">
+        <v>535</v>
+      </c>
     </row>
     <row r="136">
+      <c r="A136" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C136" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="D136" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H136" s="1" t="s">
+        <v>343</v>
+      </c>
       <c r="I136" s="30"/>
       <c r="J136" s="30"/>
       <c r="K136" s="30"/>
-      <c r="L136" s="30"/>
+      <c r="L136" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="M136" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="O136" s="1" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="137">
+      <c r="A137" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C137" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D137" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G137" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H137" s="1" t="s">
+        <v>343</v>
+      </c>
       <c r="I137" s="30"/>
       <c r="J137" s="30"/>
       <c r="K137" s="30"/>
-      <c r="L137" s="30"/>
+      <c r="L137" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="M137" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="O137" s="1" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="138">
+      <c r="A138" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C138" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="D138" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H138" s="1" t="s">
+        <v>343</v>
+      </c>
       <c r="I138" s="30"/>
       <c r="J138" s="30"/>
       <c r="K138" s="30"/>
-      <c r="L138" s="30"/>
+      <c r="L138" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="M138" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="O138" s="1" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="139">
+      <c r="A139" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C139" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="D139" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H139" s="1" t="s">
+        <v>343</v>
+      </c>
       <c r="I139" s="30"/>
       <c r="J139" s="30"/>
       <c r="K139" s="30"/>
-      <c r="L139" s="30"/>
+      <c r="L139" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="M139" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="O139" s="1" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="140">
+      <c r="A140" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C140" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="D140" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G140" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H140" s="1" t="s">
+        <v>330</v>
+      </c>
       <c r="I140" s="30"/>
       <c r="J140" s="30"/>
       <c r="K140" s="30"/>
-      <c r="L140" s="30"/>
+      <c r="L140" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="M140" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="O140" s="1" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="141">
+      <c r="A141" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C141" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="D141" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G141" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H141" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="I141" s="30"/>
       <c r="J141" s="30"/>
       <c r="K141" s="30"/>
-      <c r="L141" s="30"/>
+      <c r="L141" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="M141" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="O141" s="1" t="s">
+        <v>543</v>
+      </c>
     </row>
     <row r="142">
+      <c r="A142" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C142" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="D142" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="G142" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H142" s="1" t="s">
+        <v>330</v>
+      </c>
       <c r="I142" s="30"/>
       <c r="J142" s="30"/>
       <c r="K142" s="30"/>
-      <c r="L142" s="30"/>
+      <c r="L142" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="M142" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="O142" s="1" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="143">
+      <c r="A143" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C143" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="D143" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="G143" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H143" s="1" t="s">
+        <v>330</v>
+      </c>
       <c r="I143" s="30"/>
       <c r="J143" s="30"/>
       <c r="K143" s="30"/>
-      <c r="L143" s="30"/>
+      <c r="L143" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="M143" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="O143" s="1" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="144">
+      <c r="A144" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C144" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="D144" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H144" s="1" t="s">
+        <v>343</v>
+      </c>
       <c r="I144" s="30"/>
       <c r="J144" s="30"/>
       <c r="K144" s="30"/>
-      <c r="L144" s="30"/>
+      <c r="L144" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="M144" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="O144" s="1" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="145">
       <c r="I145" s="30"/>
@@ -14954,7 +16168,7 @@
         <v>329</v>
       </c>
       <c r="G54" s="29" t="s">
-        <v>504</v>
+        <v>547</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>350</v>
@@ -14994,7 +16208,7 @@
         <v>329</v>
       </c>
       <c r="G55" s="29" t="s">
-        <v>504</v>
+        <v>547</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>350</v>
@@ -15037,7 +16251,7 @@
         <v>329</v>
       </c>
       <c r="G56" s="29" t="s">
-        <v>504</v>
+        <v>547</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>350</v>
@@ -15077,7 +16291,7 @@
         <v>329</v>
       </c>
       <c r="G57" s="29" t="s">
-        <v>504</v>
+        <v>547</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>350</v>
@@ -15117,7 +16331,7 @@
         <v>329</v>
       </c>
       <c r="G58" s="29" t="s">
-        <v>504</v>
+        <v>547</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>350</v>
@@ -15190,7 +16404,7 @@
         <v>342</v>
       </c>
       <c r="G60" s="29" t="s">
-        <v>504</v>
+        <v>547</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>350</v>
@@ -15226,7 +16440,7 @@
         <v>342</v>
       </c>
       <c r="G61" s="29" t="s">
-        <v>504</v>
+        <v>547</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>350</v>
@@ -15262,7 +16476,7 @@
         <v>342</v>
       </c>
       <c r="G62" s="29" t="s">
-        <v>504</v>
+        <v>547</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>350</v>
@@ -15550,7 +16764,7 @@
         <v>342</v>
       </c>
       <c r="G70" s="29" t="s">
-        <v>504</v>
+        <v>547</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>350</v>
@@ -15766,7 +16980,7 @@
         <v>329</v>
       </c>
       <c r="G76" s="29" t="s">
-        <v>504</v>
+        <v>547</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>350</v>
@@ -15799,7 +17013,7 @@
         <v>329</v>
       </c>
       <c r="G77" s="29" t="s">
-        <v>504</v>
+        <v>547</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>350</v>
@@ -16868,7 +18082,7 @@
         <v>329</v>
       </c>
       <c r="G109" s="29" t="s">
-        <v>504</v>
+        <v>547</v>
       </c>
       <c r="H109" s="1" t="s">
         <v>350</v>
@@ -16908,25 +18122,25 @@
         <v>308</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>505</v>
+        <v>548</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>506</v>
+        <v>549</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>507</v>
+        <v>550</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>508</v>
+        <v>551</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>509</v>
+        <v>552</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>510</v>
+        <v>553</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>511</v>
+        <v>554</v>
       </c>
     </row>
     <row r="2">
@@ -16957,7 +18171,7 @@
     </row>
     <row r="3">
       <c r="A3" s="29" t="s">
-        <v>512</v>
+        <v>555</v>
       </c>
       <c r="B3" s="1">
         <v>1.0</v>
@@ -16971,7 +18185,7 @@
     </row>
     <row r="4">
       <c r="A4" s="29" t="s">
-        <v>513</v>
+        <v>556</v>
       </c>
       <c r="B4" s="1">
         <v>1.0</v>
@@ -17008,21 +18222,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>514</v>
+        <v>557</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>515</v>
+        <v>558</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>516</v>
+        <v>559</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>517</v>
+        <v>560</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>518</v>
+        <v>561</v>
       </c>
       <c r="B2" s="1">
         <v>1.0</v>
@@ -17036,7 +18250,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>519</v>
+        <v>562</v>
       </c>
       <c r="B3" s="1">
         <v>2.0</v>
@@ -17050,7 +18264,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>520</v>
+        <v>563</v>
       </c>
       <c r="B4" s="1">
         <v>3.0</v>
@@ -17064,7 +18278,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>521</v>
+        <v>564</v>
       </c>
       <c r="B5" s="1">
         <v>4.0</v>
@@ -17099,20 +18313,20 @@
         <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>522</v>
+        <v>565</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>523</v>
+        <v>566</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>524</v>
+        <v>567</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>525</v>
+        <v>568</v>
       </c>
       <c r="B3" s="1">
         <v>4.0</v>
@@ -17123,7 +18337,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>526</v>
+        <v>569</v>
       </c>
       <c r="B4" s="1">
         <v>4.0</v>
@@ -17134,7 +18348,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>527</v>
+        <v>570</v>
       </c>
       <c r="B5" s="1">
         <v>5.0</v>
@@ -17166,12 +18380,12 @@
         <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>528</v>
+        <v>571</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>529</v>
+        <v>572</v>
       </c>
       <c r="B2" s="1">
         <v>10.0</v>
@@ -17179,7 +18393,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>530</v>
+        <v>573</v>
       </c>
       <c r="B3" s="1">
         <v>8.0</v>
@@ -17187,7 +18401,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>531</v>
+        <v>574</v>
       </c>
       <c r="B4" s="1">
         <v>10.0</v>
@@ -17195,7 +18409,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>532</v>
+        <v>575</v>
       </c>
       <c r="B5" s="1">
         <v>6.0</v>
@@ -17221,13 +18435,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>533</v>
+        <v>576</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>534</v>
+        <v>577</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>535</v>
+        <v>578</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>78</v>
@@ -17257,22 +18471,22 @@
         <v>87</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>536</v>
+        <v>579</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>537</v>
+        <v>580</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>538</v>
+        <v>581</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>539</v>
+        <v>582</v>
       </c>
       <c r="Q1" s="9" t="s">
-        <v>540</v>
+        <v>583</v>
       </c>
       <c r="R1" s="9" t="s">
-        <v>541</v>
+        <v>584</v>
       </c>
       <c r="S1" s="9" t="s">
         <v>96</v>
@@ -17287,7 +18501,7 @@
         <v>97</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>542</v>
+        <v>585</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>101</v>
@@ -17894,13 +19108,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>533</v>
+        <v>576</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>534</v>
+        <v>577</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>535</v>
+        <v>578</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>78</v>
@@ -17930,22 +19144,22 @@
         <v>87</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>536</v>
+        <v>579</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>537</v>
+        <v>580</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>538</v>
+        <v>581</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>539</v>
+        <v>582</v>
       </c>
       <c r="Q1" s="9" t="s">
-        <v>540</v>
+        <v>583</v>
       </c>
       <c r="R1" s="9" t="s">
-        <v>541</v>
+        <v>584</v>
       </c>
       <c r="S1" s="9" t="s">
         <v>96</v>
@@ -17956,7 +19170,7 @@
         <v>97</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>543</v>
+        <v>586</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>101</v>
@@ -18347,13 +19561,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>533</v>
+        <v>576</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>534</v>
+        <v>577</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>535</v>
+        <v>578</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>78</v>
@@ -18383,22 +19597,22 @@
         <v>87</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>536</v>
+        <v>579</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>537</v>
+        <v>580</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>538</v>
+        <v>581</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>539</v>
+        <v>582</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>540</v>
+        <v>583</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>541</v>
+        <v>584</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>96</v>
@@ -18410,7 +19624,7 @@
         <v>97</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>543</v>
+        <v>586</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>101</v>
@@ -18757,7 +19971,7 @@
         <v>4.0</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>544</v>
+        <v>587</v>
       </c>
       <c r="T7" s="1"/>
     </row>
@@ -18778,13 +19992,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>533</v>
+        <v>576</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>534</v>
+        <v>577</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>535</v>
+        <v>578</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>78</v>
@@ -18814,22 +20028,22 @@
         <v>87</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>536</v>
+        <v>579</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>537</v>
+        <v>580</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>538</v>
+        <v>581</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>539</v>
+        <v>582</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>540</v>
+        <v>583</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>541</v>
+        <v>584</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>96</v>
@@ -18841,7 +20055,7 @@
         <v>97</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>543</v>
+        <v>586</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>101</v>
@@ -19213,13 +20427,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>533</v>
+        <v>576</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>534</v>
+        <v>577</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>535</v>
+        <v>578</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>78</v>
@@ -19249,22 +20463,22 @@
         <v>87</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>536</v>
+        <v>579</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>537</v>
+        <v>580</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>538</v>
+        <v>581</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>539</v>
+        <v>582</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>540</v>
+        <v>583</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>541</v>
+        <v>584</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>96</v>
@@ -19276,7 +20490,7 @@
         <v>97</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>545</v>
+        <v>588</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>101</v>
@@ -19560,7 +20774,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>546</v>
+        <v>589</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>134</v>
@@ -19620,7 +20834,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>547</v>
+        <v>590</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>153</v>

</xml_diff>